<commit_message>
🧑‍💻 ♻️ Splitted Studiengang and Ausbildungsrichtung in two enums instead of one.
</commit_message>
<xml_diff>
--- a/praktikumsplaner-backend/src/test/resources/de/muenchen/oss/praktikumsplaner/service/ExcelNwkInvalidData.xlsx
+++ b/praktikumsplaner-backend/src/test/resources/de/muenchen/oss/praktikumsplaner/service/ExcelNwkInvalidData.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis.einig\IdeaProjects\Praktikumsplaner\Praktikumsplaner\praktikumsplaner-backend\src\test\resources\de\muenchen\oss\praktikumsplaner\service\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.nischwitz\Documents\Praktikumsplaner\praktikumsplaner-backend\src\test\resources\de\muenchen\oss\praktikumsplaner\service\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB17FC2B-0A4C-4367-8AA7-7333CA9D0760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B9D748-EAE5-4B16-B1BB-5D0BAAD68A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29760" yWindow="-4470" windowWidth="28800" windowHeight="15375" xr2:uid="{E95CBEE5-BDCF-48D0-B574-A8FA4EA1B085}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E95CBEE5-BDCF-48D0-B574-A8FA4EA1B085}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -507,19 +506,19 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.796875" customWidth="1"/>
-    <col min="2" max="2" width="16.69921875" customWidth="1"/>
-    <col min="3" max="3" width="15.796875" customWidth="1"/>
-    <col min="4" max="4" width="18.09765625" customWidth="1"/>
-    <col min="5" max="5" width="20.8984375" customWidth="1"/>
+    <col min="1" max="1" width="15.75" customWidth="1"/>
+    <col min="2" max="2" width="16.75" customWidth="1"/>
+    <col min="3" max="3" width="15.75" customWidth="1"/>
+    <col min="4" max="4" width="18.125" customWidth="1"/>
+    <col min="5" max="5" width="20.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="27.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -536,7 +535,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -553,7 +552,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -566,7 +565,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -579,7 +578,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -594,7 +593,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -609,7 +608,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -624,7 +623,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -639,7 +638,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -650,7 +649,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -667,7 +666,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -684,7 +683,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Revert "🧑‍💻 ♻️ Splitted Studiengang and Ausbildungsrichtung in two enums instead of one."
This reverts commit bfb379341e9b5acde21718fae39919d41f6c6871.
</commit_message>
<xml_diff>
--- a/praktikumsplaner-backend/src/test/resources/de/muenchen/oss/praktikumsplaner/service/ExcelNwkInvalidData.xlsx
+++ b/praktikumsplaner-backend/src/test/resources/de/muenchen/oss/praktikumsplaner/service/ExcelNwkInvalidData.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.nischwitz\Documents\Praktikumsplaner\praktikumsplaner-backend\src\test\resources\de\muenchen\oss\praktikumsplaner\service\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis.einig\IdeaProjects\Praktikumsplaner\Praktikumsplaner\praktikumsplaner-backend\src\test\resources\de\muenchen\oss\praktikumsplaner\service\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B9D748-EAE5-4B16-B1BB-5D0BAAD68A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB17FC2B-0A4C-4367-8AA7-7333CA9D0760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E95CBEE5-BDCF-48D0-B574-A8FA4EA1B085}"/>
+    <workbookView xWindow="29760" yWindow="-4470" windowWidth="28800" windowHeight="15375" xr2:uid="{E95CBEE5-BDCF-48D0-B574-A8FA4EA1B085}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -506,19 +507,19 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.75" customWidth="1"/>
-    <col min="2" max="2" width="16.75" customWidth="1"/>
-    <col min="3" max="3" width="15.75" customWidth="1"/>
-    <col min="4" max="4" width="18.125" customWidth="1"/>
-    <col min="5" max="5" width="20.875" customWidth="1"/>
+    <col min="1" max="1" width="15.796875" customWidth="1"/>
+    <col min="2" max="2" width="16.69921875" customWidth="1"/>
+    <col min="3" max="3" width="15.796875" customWidth="1"/>
+    <col min="4" max="4" width="18.09765625" customWidth="1"/>
+    <col min="5" max="5" width="20.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -535,7 +536,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -552,7 +553,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -565,7 +566,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -578,7 +579,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -593,7 +594,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -608,7 +609,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -623,7 +624,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -638,7 +639,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -649,7 +650,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -666,7 +667,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -683,7 +684,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Revert "Revert "🧑‍💻 ♻️ Splitted Studiengang and Ausbildungsrichtung in two enums instead of one.""
This reverts commit 6316177a568e9e70b9d43d9118e1f5d79f866741.
</commit_message>
<xml_diff>
--- a/praktikumsplaner-backend/src/test/resources/de/muenchen/oss/praktikumsplaner/service/ExcelNwkInvalidData.xlsx
+++ b/praktikumsplaner-backend/src/test/resources/de/muenchen/oss/praktikumsplaner/service/ExcelNwkInvalidData.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis.einig\IdeaProjects\Praktikumsplaner\Praktikumsplaner\praktikumsplaner-backend\src\test\resources\de\muenchen\oss\praktikumsplaner\service\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.nischwitz\Documents\Praktikumsplaner\praktikumsplaner-backend\src\test\resources\de\muenchen\oss\praktikumsplaner\service\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB17FC2B-0A4C-4367-8AA7-7333CA9D0760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B9D748-EAE5-4B16-B1BB-5D0BAAD68A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29760" yWindow="-4470" windowWidth="28800" windowHeight="15375" xr2:uid="{E95CBEE5-BDCF-48D0-B574-A8FA4EA1B085}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E95CBEE5-BDCF-48D0-B574-A8FA4EA1B085}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -507,19 +506,19 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.796875" customWidth="1"/>
-    <col min="2" max="2" width="16.69921875" customWidth="1"/>
-    <col min="3" max="3" width="15.796875" customWidth="1"/>
-    <col min="4" max="4" width="18.09765625" customWidth="1"/>
-    <col min="5" max="5" width="20.8984375" customWidth="1"/>
+    <col min="1" max="1" width="15.75" customWidth="1"/>
+    <col min="2" max="2" width="16.75" customWidth="1"/>
+    <col min="3" max="3" width="15.75" customWidth="1"/>
+    <col min="4" max="4" width="18.125" customWidth="1"/>
+    <col min="5" max="5" width="20.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="27.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -536,7 +535,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -553,7 +552,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -566,7 +565,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -579,7 +578,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>8</v>
@@ -594,7 +593,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -609,7 +608,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -624,7 +623,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -639,7 +638,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -650,7 +649,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -667,7 +666,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -684,7 +683,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>